<commit_message>
added Swedish language index for Performance and Reflection palettes added Spanish translation for Reflection palette
</commit_message>
<xml_diff>
--- a/mod/z02_clipit_api/libraries/reflection_palette/reflection_palette_es.xlsx
+++ b/mod/z02_clipit_api/libraries/reflection_palette/reflection_palette_es.xlsx
@@ -44,91 +44,91 @@
     <t>category_description</t>
   </si>
   <si>
-    <t>One term refers to multiple concepts</t>
-  </si>
-  <si>
-    <t>One scientific term has a different meaning depending on the context it is used in. e.g. volts and voltage in Physics. Use of the term kinetic energy in both Physics and in Biology.</t>
-  </si>
-  <si>
-    <t>Terminology</t>
-  </si>
-  <si>
-    <t>Problems with use of language and scientific terms, inconsistent and overlapping terminology.</t>
-  </si>
-  <si>
-    <t>One concept has many scientific names</t>
-  </si>
-  <si>
-    <t>Different terms are used to refer to the same concept. e.g. voltage is also referred to as potential difference. Confusion between voltage and charge.</t>
-  </si>
-  <si>
-    <t>Understanding of Scientific method, process and practice</t>
-  </si>
-  <si>
-    <t>Previous understandings that need to be unlearned, modified or improved to understand the Tricky Topic</t>
-  </si>
-  <si>
-    <t>Scientific use of everyday language</t>
-  </si>
-  <si>
-    <t>Everyday terms that students reused in a scientific context, where their scientific meaning may be slightly different to that understood by students.e.g. in Physics, the “drop” part of “forward voltage drop”, "current" related to electricity and  "requency", relating to waves. Use of the word "proof" to mean evidence.</t>
-  </si>
-  <si>
-    <t>Obscure scientific terminology</t>
-  </si>
-  <si>
-    <t>Scientific terms that are simply hard for students to remember.</t>
-  </si>
-  <si>
-    <t>Simplistic understandings that may need to be unlearned or revised e.g. imagining atomic structure as balls on sticks suggests space between atoms. Belief that only 50% of parent DNA is passed on to a child. Previous knowledge schemes that need to be modified to integrate new knowledge.</t>
-  </si>
-  <si>
-    <t>Incomplete pre-knowledge</t>
-  </si>
-  <si>
-    <t>Underpinning understandings</t>
-  </si>
-  <si>
-    <t>Understanding that the student is expected to know already. e.g. to do the calculations related to Avogadro’s number in Chemistry assumes a math understanding of powers of ten and ratios. Learning about genetic drift assumes an understanding of natural selection.</t>
-  </si>
-  <si>
-    <t>Essential Concepts</t>
-  </si>
-  <si>
-    <t>Complementary concepts that the student needs to learn alongside the topic in order to make sense of the new knowledge. e.g. understanding genetic drift involves learning about its causes; founder effect and bottleneck effect.</t>
-  </si>
-  <si>
-    <t>Complementary concepts</t>
-  </si>
-  <si>
-    <t>Key assumptions and knowledge that relate to the tricky topic, without which it is impossible to understand it</t>
-  </si>
-  <si>
-    <t>Weak human-like or world-like analogy</t>
-  </si>
-  <si>
-    <t>Human-Like or world like analogy. Viewing scientific concepts in terms of everyday phenomena e.g. males of any species are bigger than females. Plants suck up food from soil thru roots.Analogy based on metaphor that doesn’t carry through e.g. “Stage” and “Costume” used in Sense programming.</t>
-  </si>
-  <si>
-    <t>Intuitive Beliefs</t>
-  </si>
-  <si>
-    <t>Informal, intuitive ways of thinking about the world. Strongly biased toward causal explanations</t>
-  </si>
-  <si>
-    <t>Key characteristic conveys group membership</t>
-  </si>
-  <si>
-    <t>The belief that if one condition is fulfilled, then the object is automatically a member of a groupOne unobservable core feature defines membership of a category eg: one to one relationship between DNA and physical traits. Birds have wings therefore all creatures with wings are birds.</t>
-  </si>
-  <si>
-    <t>Flawed causal reasoning</t>
-  </si>
-  <si>
-    <t>Reasononing based on the assumption of goal or purpose eg birds have wings so they can fly. Genes turn off in order to enable a cell to develop properly. Inappropriate assumption of cause and effect, eg release an object along a curved path and it will continue in a curve, rocks are pointy so that animals won’t sit on them and crush them.</t>
-  </si>
-  <si>
     <t>es</t>
+  </si>
+  <si>
+    <t>Un mismo término hace referencia a múltiples conceptos</t>
+  </si>
+  <si>
+    <t>Un mismo concepto tiene varios nombres científicos</t>
+  </si>
+  <si>
+    <t>Expresiones coloquiales para conceptos científicos</t>
+  </si>
+  <si>
+    <t>Terminología científica compleja</t>
+  </si>
+  <si>
+    <t>Comprensión del método científico, el proceso y la práctica</t>
+  </si>
+  <si>
+    <t>Conocimiento subyacente</t>
+  </si>
+  <si>
+    <t>Conceptos esenciales</t>
+  </si>
+  <si>
+    <t>Asociación a un grupo por característica clave en común</t>
+  </si>
+  <si>
+    <t>Razonamiento casual incorrecto</t>
+  </si>
+  <si>
+    <t>Un término científico tiene varios significados dependiendo del contexto en que se usa. Por ejemplo: 'voltios' y 'voltaje' en física, o el uso de 'kinética' en física o biología.</t>
+  </si>
+  <si>
+    <t>Distintos términos se pueden usar para referirse a un mismo concepto. Por ejemplo: 'voltaje' también se puede llamar 'diferencia potencial', o la confusión entre 'voltaje' y 'carga'.</t>
+  </si>
+  <si>
+    <t>Términos coloquiales ue los estudiantes usan en un contexto científico, donde su significado científico puede ser ligeramente distinto que el entendido por los estudiantes. Por ejemplo: en física, la palabra 'caída' en 'caída de tensión'; la palabra 'corriente' refiriéndose a electricidad; la palabra 'frecuencia', refiriéndose a ondas; o la palabra 'pruebas' para referirse a 'evidencia'.</t>
+  </si>
+  <si>
+    <t>Terminología</t>
+  </si>
+  <si>
+    <t>Conceptos complementarios</t>
+  </si>
+  <si>
+    <t>Creencias intuitivas</t>
+  </si>
+  <si>
+    <t>Falta de conocimientos previos</t>
+  </si>
+  <si>
+    <t>Conceptos clave y conocimiento que está relacionado con un tema, y sin los cuales es imposible comprenderlo.</t>
+  </si>
+  <si>
+    <t>Conocimientos previos que deben ser omitidos, alterados o mejorados para comprender un tema.</t>
+  </si>
+  <si>
+    <t>Problemas con el uso del lenguaje y de los términos científicos, inconsistentemente y solapando la terminología.</t>
+  </si>
+  <si>
+    <t>Formas de entender conceptos globales que son informales o intuitivas. Opiniones parciales debidas a explicaciones casuales.</t>
+  </si>
+  <si>
+    <t>Términos científicos que son dificiles de recordar para estudiantes.</t>
+  </si>
+  <si>
+    <t>Conocimiento simplísta que requiere ser omitido o revisado. Por ejemplo: imaginar la estructura atómica como bolas en palos sugiere que hay huecos entre los átomos; o creer que sólo el 50% del ADN de cada padre es heredado por el hijo. Esquemas de conocimiento previo que necesitan ser modificados para adaptar nuevo conocimiento.</t>
+  </si>
+  <si>
+    <t>Conocimiento que se espera que el estudiante sepa de antemano. Por ejemplo: para realizar cálculos relacionados con el número de Avogadro en química, se asume un conocimiento matemático de potencias y relaciones; o aprendiendo acerca de la deriva genética, se asume un conocimiento sobre selección natural.</t>
+  </si>
+  <si>
+    <t>Conceptos complementarios que un estudiante necesita aprender a la vez que el tema en cuestion, de cara a dar sentido a los nuevos conocimientos. Por ejemplo:  entender la deriva genética involucra aprender sus causas; o  entender el efecto fundador involucra entender el efecto cuello de botella.</t>
+  </si>
+  <si>
+    <t>Analogía humana o del entorno muy pobre</t>
+  </si>
+  <si>
+    <t>Analogías al ser humano o al medio natural. Comprender conceptos científicos en términos de fenómenos cotidianos. Por ejemplo: los machos de cualquier especie son más grandes que las hembras; o las plantas cogen alimento desde la tierra a través de sus raíces. Metáforas basadas en analogías que no son consistentes. Por ejemplo: 'escenario' y 'disfraz' en programación sensorial.</t>
+  </si>
+  <si>
+    <t>La creencia de que, si una característica clave se cumple, entonces el individuo es parte de una colección preestablecida. Por ejemplo: que existe una relación uno-a-uno entre genes del AND y rasgos físicos; o que como los pájaros tienen alas y vuelan, todas las criaturas con alas vuelan.</t>
+  </si>
+  <si>
+    <t>Razonamiento basado en supuestos objetivos o propósitos. Por ejemplo: que los pájaros tienen alas para poder volar; o que los genes se desactivan para permitir que las células se desarrollen adecuadamente. Supuestos inapropiados de causa y efecto. Por ejemplo: que si se libera un objeto en un camino curvo, el objeto seguirá la trayectoria; o que las rocas son puntiagudas para que los animales no se puedan sentar encima y romperlas.</t>
   </si>
 </sst>
 </file>
@@ -451,19 +451,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="39.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="41.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="39.5703125" style="1"/>
+    <col min="3" max="3" width="54.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.140625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="41.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -486,204 +486,204 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>